<commit_message>
make some docstrings and comments
</commit_message>
<xml_diff>
--- a/BattleScript/table.xlsx
+++ b/BattleScript/table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{086E7B3F-F930-4B00-91F5-CA5C137C6300}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{714ABB95-7ECC-4415-B340-CA0995A8A8F5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -322,20 +322,20 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -620,7 +620,7 @@
   <dimension ref="B1:Y52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="N41" sqref="N41"/>
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,55 +648,55 @@
   <sheetData>
     <row r="1" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="1"/>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="N1" s="14" t="s">
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="N1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
       <c r="V1" s="4"/>
-      <c r="W1" s="13" t="s">
+      <c r="W1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="13"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
     </row>
     <row r="2" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="1"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14"/>
-      <c r="T2" s="14"/>
-      <c r="U2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
       <c r="V2" s="4"/>
-      <c r="W2" s="13"/>
-      <c r="X2" s="13"/>
-      <c r="Y2" s="13"/>
+      <c r="W2" s="14"/>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
     </row>
     <row r="3" spans="2:25" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -1480,24 +1480,24 @@
       <c r="X36" s="16"/>
     </row>
     <row r="37" spans="2:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C37" s="15" t="s">
+      <c r="C37" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="15"/>
-      <c r="N37" s="15" t="s">
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="17"/>
+      <c r="N37" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="O37" s="15"/>
-      <c r="P37" s="15"/>
-      <c r="Q37" s="15"/>
-      <c r="R37" s="15"/>
-      <c r="S37" s="15"/>
-      <c r="T37" s="15"/>
+      <c r="O37" s="17"/>
+      <c r="P37" s="17"/>
+      <c r="Q37" s="17"/>
+      <c r="R37" s="17"/>
+      <c r="S37" s="17"/>
+      <c r="T37" s="17"/>
       <c r="W37" s="11" t="s">
         <v>59</v>
       </c>
@@ -1506,20 +1506,20 @@
       </c>
     </row>
     <row r="38" spans="2:24" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="15"/>
-      <c r="I38" s="15"/>
-      <c r="N38" s="15"/>
-      <c r="O38" s="15"/>
-      <c r="P38" s="15"/>
-      <c r="Q38" s="15"/>
-      <c r="R38" s="15"/>
-      <c r="S38" s="15"/>
-      <c r="T38" s="15"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="17"/>
+      <c r="N38" s="17"/>
+      <c r="O38" s="17"/>
+      <c r="P38" s="17"/>
+      <c r="Q38" s="17"/>
+      <c r="R38" s="17"/>
+      <c r="S38" s="17"/>
+      <c r="T38" s="17"/>
       <c r="W38" s="12" t="s">
         <v>58</v>
       </c>
@@ -1528,20 +1528,20 @@
       </c>
     </row>
     <row r="39" spans="2:24" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C39" s="15"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="15"/>
-      <c r="F39" s="15"/>
-      <c r="G39" s="15"/>
-      <c r="H39" s="15"/>
-      <c r="I39" s="15"/>
-      <c r="N39" s="15"/>
-      <c r="O39" s="15"/>
-      <c r="P39" s="15"/>
-      <c r="Q39" s="15"/>
-      <c r="R39" s="15"/>
-      <c r="S39" s="15"/>
-      <c r="T39" s="15"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="17"/>
+      <c r="N39" s="17"/>
+      <c r="O39" s="17"/>
+      <c r="P39" s="17"/>
+      <c r="Q39" s="17"/>
+      <c r="R39" s="17"/>
+      <c r="S39" s="17"/>
+      <c r="T39" s="17"/>
       <c r="W39" s="12" t="s">
         <v>57</v>
       </c>
@@ -1574,8 +1574,8 @@
       <c r="Q40" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="R40" s="17"/>
-      <c r="S40" s="17"/>
+      <c r="R40" s="13"/>
+      <c r="S40" s="13"/>
       <c r="W40" s="12" t="s">
         <v>54</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>500</v>
       </c>
       <c r="E41" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F41" s="8" t="s">
         <v>33</v>
@@ -1603,13 +1603,13 @@
         <v>36</v>
       </c>
       <c r="O41" s="5">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="P41" s="5">
         <v>5</v>
       </c>
       <c r="Q41" s="8" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="R41" s="10"/>
       <c r="S41" s="10"/>

</xml_diff>

<commit_message>
refactor for replace lists to dicts and add unit names in army lists
</commit_message>
<xml_diff>
--- a/BattleScript/table.xlsx
+++ b/BattleScript/table.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{714ABB95-7ECC-4415-B340-CA0995A8A8F5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47871C21-4E75-4206-B01A-594C76C87626}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -619,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Y52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,7 +761,7 @@
       </c>
     </row>
     <row r="4" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -788,7 +788,7 @@
       <c r="J4" s="5">
         <v>2</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="5" t="s">
         <v>10</v>
       </c>
       <c r="N4" s="5" t="s">
@@ -823,7 +823,7 @@
       </c>
     </row>
     <row r="5" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="5" t="s">
@@ -850,7 +850,7 @@
       <c r="J5" s="5">
         <v>2</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="5" t="s">
         <v>22</v>
       </c>
       <c r="N5" s="5" t="s">
@@ -885,7 +885,7 @@
       </c>
     </row>
     <row r="6" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -912,6 +912,7 @@
       <c r="J6" s="5">
         <v>2</v>
       </c>
+      <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
@@ -928,6 +929,7 @@
       </c>
     </row>
     <row r="7" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -936,6 +938,7 @@
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
+      <c r="M7" s="5"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
@@ -952,6 +955,7 @@
       </c>
     </row>
     <row r="8" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
@@ -960,6 +964,7 @@
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
+      <c r="M8" s="5"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
@@ -976,6 +981,7 @@
       </c>
     </row>
     <row r="9" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
@@ -984,6 +990,7 @@
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
+      <c r="M9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
@@ -1000,6 +1007,7 @@
       </c>
     </row>
     <row r="10" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -1008,6 +1016,7 @@
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
+      <c r="M10" s="5"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
@@ -1024,6 +1033,7 @@
       </c>
     </row>
     <row r="11" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -1032,6 +1042,7 @@
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
+      <c r="M11" s="5"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
@@ -1042,6 +1053,7 @@
       <c r="U11" s="5"/>
     </row>
     <row r="12" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -1050,6 +1062,7 @@
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
+      <c r="M12" s="5"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
@@ -1060,6 +1073,7 @@
       <c r="U12" s="5"/>
     </row>
     <row r="13" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
@@ -1068,6 +1082,7 @@
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
+      <c r="M13" s="5"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
@@ -1078,6 +1093,7 @@
       <c r="U13" s="5"/>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -1086,6 +1102,7 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
+      <c r="M14" s="5"/>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
@@ -1096,6 +1113,7 @@
       <c r="U14" s="5"/>
     </row>
     <row r="15" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -1104,6 +1122,7 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
+      <c r="M15" s="5"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
@@ -1114,6 +1133,7 @@
       <c r="U15" s="5"/>
     </row>
     <row r="16" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -1122,6 +1142,7 @@
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
+      <c r="M16" s="5"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
@@ -1131,7 +1152,8 @@
       <c r="T16" s="5"/>
       <c r="U16" s="5"/>
     </row>
-    <row r="17" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -1140,6 +1162,7 @@
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
+      <c r="M17" s="5"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
@@ -1149,7 +1172,8 @@
       <c r="T17" s="5"/>
       <c r="U17" s="5"/>
     </row>
-    <row r="18" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -1158,6 +1182,7 @@
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
+      <c r="M18" s="5"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
@@ -1167,7 +1192,8 @@
       <c r="T18" s="5"/>
       <c r="U18" s="5"/>
     </row>
-    <row r="19" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -1176,6 +1202,7 @@
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
+      <c r="M19" s="5"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
@@ -1185,7 +1212,8 @@
       <c r="T19" s="5"/>
       <c r="U19" s="5"/>
     </row>
-    <row r="20" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
@@ -1194,6 +1222,7 @@
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
+      <c r="M20" s="5"/>
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
       <c r="P20" s="5"/>
@@ -1203,7 +1232,8 @@
       <c r="T20" s="5"/>
       <c r="U20" s="5"/>
     </row>
-    <row r="21" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
@@ -1212,6 +1242,7 @@
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
+      <c r="M21" s="5"/>
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
       <c r="P21" s="5"/>
@@ -1221,7 +1252,8 @@
       <c r="T21" s="5"/>
       <c r="U21" s="5"/>
     </row>
-    <row r="22" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
@@ -1230,6 +1262,7 @@
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
+      <c r="M22" s="5"/>
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
       <c r="P22" s="5"/>
@@ -1239,7 +1272,8 @@
       <c r="T22" s="5"/>
       <c r="U22" s="5"/>
     </row>
-    <row r="23" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
@@ -1248,6 +1282,7 @@
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
+      <c r="M23" s="5"/>
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
       <c r="P23" s="5"/>
@@ -1257,7 +1292,8 @@
       <c r="T23" s="5"/>
       <c r="U23" s="5"/>
     </row>
-    <row r="24" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
@@ -1266,6 +1302,7 @@
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
+      <c r="M24" s="5"/>
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
       <c r="P24" s="5"/>
@@ -1275,7 +1312,8 @@
       <c r="T24" s="5"/>
       <c r="U24" s="5"/>
     </row>
-    <row r="25" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
@@ -1284,6 +1322,7 @@
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
+      <c r="M25" s="5"/>
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
       <c r="P25" s="5"/>
@@ -1293,7 +1332,8 @@
       <c r="T25" s="5"/>
       <c r="U25" s="5"/>
     </row>
-    <row r="26" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
@@ -1302,6 +1342,7 @@
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
+      <c r="M26" s="5"/>
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
       <c r="P26" s="5"/>
@@ -1311,7 +1352,8 @@
       <c r="T26" s="5"/>
       <c r="U26" s="5"/>
     </row>
-    <row r="27" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
@@ -1320,6 +1362,7 @@
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
+      <c r="M27" s="5"/>
       <c r="N27" s="5"/>
       <c r="O27" s="5"/>
       <c r="P27" s="5"/>
@@ -1329,7 +1372,8 @@
       <c r="T27" s="5"/>
       <c r="U27" s="5"/>
     </row>
-    <row r="28" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
@@ -1338,6 +1382,7 @@
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
+      <c r="M28" s="5"/>
       <c r="N28" s="5"/>
       <c r="O28" s="5"/>
       <c r="P28" s="5"/>
@@ -1347,7 +1392,8 @@
       <c r="T28" s="5"/>
       <c r="U28" s="5"/>
     </row>
-    <row r="29" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
@@ -1356,6 +1402,7 @@
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
+      <c r="M29" s="5"/>
       <c r="N29" s="5"/>
       <c r="O29" s="5"/>
       <c r="P29" s="5"/>
@@ -1365,7 +1412,8 @@
       <c r="T29" s="5"/>
       <c r="U29" s="5"/>
     </row>
-    <row r="30" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
@@ -1374,6 +1422,7 @@
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
+      <c r="M30" s="5"/>
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
       <c r="P30" s="5"/>
@@ -1383,7 +1432,8 @@
       <c r="T30" s="5"/>
       <c r="U30" s="5"/>
     </row>
-    <row r="31" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
@@ -1392,6 +1442,7 @@
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
+      <c r="M31" s="5"/>
       <c r="N31" s="5"/>
       <c r="O31" s="5"/>
       <c r="P31" s="5"/>
@@ -1401,7 +1452,8 @@
       <c r="T31" s="5"/>
       <c r="U31" s="5"/>
     </row>
-    <row r="32" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
@@ -1410,6 +1462,7 @@
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
+      <c r="M32" s="5"/>
       <c r="N32" s="5"/>
       <c r="O32" s="5"/>
       <c r="P32" s="5"/>
@@ -1420,6 +1473,7 @@
       <c r="U32" s="5"/>
     </row>
     <row r="33" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
@@ -1428,6 +1482,7 @@
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
+      <c r="M33" s="5"/>
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
       <c r="P33" s="5"/>
@@ -1438,6 +1493,7 @@
       <c r="U33" s="5"/>
     </row>
     <row r="34" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
@@ -1446,6 +1502,7 @@
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
+      <c r="M34" s="5"/>
       <c r="N34" s="5"/>
       <c r="O34" s="5"/>
       <c r="P34" s="5"/>
@@ -1456,6 +1513,7 @@
       <c r="U34" s="5"/>
     </row>
     <row r="35" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
@@ -1464,6 +1522,7 @@
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
+      <c r="M35" s="5"/>
       <c r="N35" s="5"/>
       <c r="O35" s="5"/>
       <c r="P35" s="5"/>
@@ -1594,7 +1653,7 @@
         <v>500</v>
       </c>
       <c r="E41" s="5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F41" s="8" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
refactor some function to "dry" principle. Not consistent version
</commit_message>
<xml_diff>
--- a/BattleScript/table.xlsx
+++ b/BattleScript/table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47871C21-4E75-4206-B01A-594C76C87626}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2CAA21-2FE2-4BB1-81C2-A549B2386DB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="64">
   <si>
     <t>Армия первая</t>
   </si>
@@ -206,6 +206,12 @@
   </si>
   <si>
     <t>Тип магии / способн.</t>
+  </si>
+  <si>
+    <t>Буря</t>
+  </si>
+  <si>
+    <t>Говно</t>
   </si>
 </sst>
 </file>
@@ -619,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Y52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="P45" sqref="P45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1609,6 +1615,9 @@
       </c>
     </row>
     <row r="40" spans="2:24" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>9</v>
+      </c>
       <c r="C40" s="2" t="s">
         <v>61</v>
       </c>
@@ -1620,6 +1629,9 @@
       </c>
       <c r="F40" s="2" t="s">
         <v>46</v>
+      </c>
+      <c r="M40" t="s">
+        <v>9</v>
       </c>
       <c r="N40" s="2" t="s">
         <v>60</v>
@@ -1653,11 +1665,14 @@
         <v>500</v>
       </c>
       <c r="E41" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F41" s="8" t="s">
         <v>33</v>
       </c>
+      <c r="M41" s="5" t="s">
+        <v>62</v>
+      </c>
       <c r="N41" s="5" t="s">
         <v>36</v>
       </c>
@@ -1665,7 +1680,7 @@
         <v>300</v>
       </c>
       <c r="P41" s="5">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="Q41" s="8" t="s">
         <v>36</v>
@@ -1690,11 +1705,14 @@
         <v>15</v>
       </c>
       <c r="E42" s="5">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F42" s="8" t="s">
         <v>14</v>
       </c>
+      <c r="M42" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="N42" s="5" t="s">
         <v>16</v>
       </c>
@@ -1702,7 +1720,7 @@
         <v>15</v>
       </c>
       <c r="P42" s="5">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="Q42" s="8" t="s">
         <v>14</v>
@@ -1721,6 +1739,7 @@
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
+      <c r="M43" s="5"/>
       <c r="N43" s="5"/>
       <c r="O43" s="5"/>
       <c r="P43" s="5"/>
@@ -1739,6 +1758,7 @@
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
+      <c r="M44" s="5"/>
       <c r="N44" s="5"/>
       <c r="O44" s="5"/>
       <c r="P44" s="5"/>
@@ -1757,6 +1777,7 @@
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
+      <c r="M45" s="5"/>
       <c r="N45" s="5"/>
       <c r="O45" s="5"/>
       <c r="P45" s="5"/>
@@ -1771,6 +1792,7 @@
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
+      <c r="M46" s="5"/>
       <c r="N46" s="5"/>
       <c r="O46" s="5"/>
       <c r="P46" s="5"/>
@@ -1785,6 +1807,7 @@
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
+      <c r="M47" s="5"/>
       <c r="N47" s="5"/>
       <c r="O47" s="5"/>
       <c r="P47" s="5"/>
@@ -1799,6 +1822,7 @@
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
+      <c r="M48" s="5"/>
       <c r="N48" s="5"/>
       <c r="O48" s="5"/>
       <c r="P48" s="5"/>
@@ -1811,6 +1835,7 @@
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
+      <c r="M49" s="5"/>
       <c r="N49" s="5"/>
       <c r="O49" s="5"/>
       <c r="P49" s="5"/>
@@ -1829,6 +1854,7 @@
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
+      <c r="M50" s="5"/>
       <c r="N50" s="5"/>
       <c r="O50" s="5"/>
       <c r="P50" s="5"/>
@@ -1847,6 +1873,7 @@
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
+      <c r="M51" s="5"/>
       <c r="N51" s="5"/>
       <c r="O51" s="5"/>
       <c r="P51" s="5"/>

</xml_diff>

<commit_message>
add magic and abil stage
</commit_message>
<xml_diff>
--- a/BattleScript/table.xlsx
+++ b/BattleScript/table.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2CAA21-2FE2-4BB1-81C2-A549B2386DB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="65">
   <si>
     <t>Армия первая</t>
   </si>
@@ -212,12 +211,15 @@
   </si>
   <si>
     <t>Говно</t>
+  </si>
+  <si>
+    <t>Бонус к комбатке</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -300,7 +302,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -330,6 +332,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -622,11 +627,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:Y52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:AA52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="P45" sqref="P45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,74 +642,80 @@
     <col min="6" max="6" width="16" customWidth="1"/>
     <col min="7" max="7" width="13.140625" customWidth="1"/>
     <col min="9" max="9" width="17.42578125" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1"/>
-    <col min="11" max="11" width="4.28515625" customWidth="1"/>
-    <col min="12" max="12" width="4.7109375" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" customWidth="1"/>
-    <col min="15" max="16" width="10" customWidth="1"/>
-    <col min="17" max="17" width="17.140625" customWidth="1"/>
-    <col min="18" max="19" width="12.5703125" customWidth="1"/>
-    <col min="20" max="20" width="14.85546875" customWidth="1"/>
-    <col min="21" max="21" width="13.42578125" customWidth="1"/>
-    <col min="22" max="22" width="3.85546875" customWidth="1"/>
-    <col min="23" max="23" width="15.28515625" customWidth="1"/>
-    <col min="24" max="24" width="12" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" customWidth="1"/>
+    <col min="12" max="12" width="4.28515625" customWidth="1"/>
+    <col min="13" max="13" width="4.7109375" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" customWidth="1"/>
+    <col min="15" max="15" width="9.7109375" customWidth="1"/>
+    <col min="16" max="17" width="10" customWidth="1"/>
+    <col min="18" max="18" width="17.140625" customWidth="1"/>
+    <col min="19" max="20" width="12.5703125" customWidth="1"/>
+    <col min="21" max="21" width="9.7109375" customWidth="1"/>
+    <col min="22" max="22" width="14.85546875" customWidth="1"/>
+    <col min="23" max="23" width="13.42578125" customWidth="1"/>
+    <col min="24" max="24" width="3.85546875" customWidth="1"/>
+    <col min="25" max="25" width="15.28515625" customWidth="1"/>
+    <col min="26" max="26" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="1"/>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="N1" s="15" t="s">
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="O1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="14" t="s">
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-    </row>
-    <row r="2" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="Z1" s="15"/>
+      <c r="AA1" s="15"/>
+    </row>
+    <row r="2" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="1"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
-      <c r="T2" s="15"/>
-      <c r="U2" s="15"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="14"/>
-      <c r="X2" s="14"/>
-      <c r="Y2" s="14"/>
-    </row>
-    <row r="3" spans="2:25" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="16"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="15"/>
+      <c r="AA2" s="15"/>
+    </row>
+    <row r="3" spans="2:27" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>9</v>
       </c>
@@ -729,44 +740,50 @@
       <c r="I3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>1</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>3</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="U3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="U3" s="2" t="s">
+      <c r="V3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="W3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="X3" s="6" t="s">
+      <c r="Z3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="Y3" s="6" t="s">
+      <c r="AA3" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
@@ -792,43 +809,49 @@
         <v>15</v>
       </c>
       <c r="J4" s="5">
+        <v>0</v>
+      </c>
+      <c r="K4" s="5">
         <v>2</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="N4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="O4" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="O4" s="5">
-        <v>100</v>
       </c>
       <c r="P4" s="5">
         <v>100</v>
       </c>
       <c r="Q4" s="5">
+        <v>100</v>
+      </c>
+      <c r="R4" s="5">
         <v>15</v>
       </c>
-      <c r="R4" s="5">
+      <c r="S4" s="5">
         <v>25</v>
       </c>
-      <c r="S4" s="5">
+      <c r="T4" s="5">
         <v>15</v>
       </c>
-      <c r="T4" s="5" t="s">
+      <c r="U4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="U4" s="5">
+      <c r="V4" s="5">
+        <v>0</v>
+      </c>
+      <c r="W4" s="5">
         <v>2</v>
       </c>
-      <c r="X4" s="6" t="s">
+      <c r="Z4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="Y4" s="6" t="s">
+      <c r="AA4" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
@@ -854,43 +877,49 @@
         <v>21</v>
       </c>
       <c r="J5" s="5">
+        <v>0</v>
+      </c>
+      <c r="K5" s="5">
         <v>2</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="N5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="O5" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="O5" s="5">
-        <v>200</v>
       </c>
       <c r="P5" s="5">
         <v>200</v>
       </c>
       <c r="Q5" s="5">
+        <v>200</v>
+      </c>
+      <c r="R5" s="5">
         <v>20</v>
       </c>
-      <c r="R5" s="5">
+      <c r="S5" s="5">
         <v>25</v>
       </c>
-      <c r="S5" s="5">
+      <c r="T5" s="5">
         <v>20</v>
       </c>
-      <c r="T5" s="5" t="s">
+      <c r="U5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="U5" s="5">
+      <c r="V5" s="5">
+        <v>0</v>
+      </c>
+      <c r="W5" s="5">
         <v>10</v>
       </c>
-      <c r="X5" s="6" t="s">
+      <c r="Z5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="Y5" s="6" t="s">
+      <c r="AA5" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>23</v>
       </c>
@@ -916,9 +945,11 @@
         <v>32</v>
       </c>
       <c r="J6" s="5">
+        <v>0</v>
+      </c>
+      <c r="K6" s="5">
         <v>2</v>
       </c>
-      <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
@@ -927,14 +958,16 @@
       <c r="S6" s="5"/>
       <c r="T6" s="5"/>
       <c r="U6" s="5"/>
-      <c r="X6" s="6" t="s">
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="Z6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="Y6" s="6" t="s">
+      <c r="AA6" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -944,7 +977,7 @@
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
-      <c r="M7" s="5"/>
+      <c r="K7" s="5"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
@@ -953,14 +986,16 @@
       <c r="S7" s="5"/>
       <c r="T7" s="5"/>
       <c r="U7" s="5"/>
-      <c r="X7" s="6" t="s">
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="Z7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="Y7" s="6" t="s">
+      <c r="AA7" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -970,7 +1005,7 @@
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
-      <c r="M8" s="5"/>
+      <c r="K8" s="5"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
@@ -979,14 +1014,16 @@
       <c r="S8" s="5"/>
       <c r="T8" s="5"/>
       <c r="U8" s="5"/>
-      <c r="X8" s="6" t="s">
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="Z8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="Y8" s="6" t="s">
+      <c r="AA8" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -996,7 +1033,7 @@
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
-      <c r="M9" s="5"/>
+      <c r="K9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
@@ -1005,14 +1042,16 @@
       <c r="S9" s="5"/>
       <c r="T9" s="5"/>
       <c r="U9" s="5"/>
-      <c r="X9" s="6" t="s">
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+      <c r="Z9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="Y9" s="6" t="s">
+      <c r="AA9" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -1022,7 +1061,7 @@
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
-      <c r="M10" s="5"/>
+      <c r="K10" s="5"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
@@ -1031,14 +1070,16 @@
       <c r="S10" s="5"/>
       <c r="T10" s="5"/>
       <c r="U10" s="5"/>
-      <c r="X10" s="6" t="s">
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+      <c r="Z10" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="Y10" s="6" t="s">
+      <c r="AA10" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -1048,7 +1089,7 @@
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
-      <c r="M11" s="5"/>
+      <c r="K11" s="5"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
@@ -1057,8 +1098,10 @@
       <c r="S11" s="5"/>
       <c r="T11" s="5"/>
       <c r="U11" s="5"/>
-    </row>
-    <row r="12" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+    </row>
+    <row r="12" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -1068,7 +1111,7 @@
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
-      <c r="M12" s="5"/>
+      <c r="K12" s="5"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
@@ -1077,8 +1120,10 @@
       <c r="S12" s="5"/>
       <c r="T12" s="5"/>
       <c r="U12" s="5"/>
-    </row>
-    <row r="13" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="V12" s="5"/>
+      <c r="W12" s="5"/>
+    </row>
+    <row r="13" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -1088,7 +1133,7 @@
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
-      <c r="M13" s="5"/>
+      <c r="K13" s="5"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
@@ -1097,8 +1142,10 @@
       <c r="S13" s="5"/>
       <c r="T13" s="5"/>
       <c r="U13" s="5"/>
-    </row>
-    <row r="14" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="V13" s="5"/>
+      <c r="W13" s="5"/>
+    </row>
+    <row r="14" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -1108,7 +1155,7 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
-      <c r="M14" s="5"/>
+      <c r="K14" s="5"/>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
@@ -1117,8 +1164,10 @@
       <c r="S14" s="5"/>
       <c r="T14" s="5"/>
       <c r="U14" s="5"/>
-    </row>
-    <row r="15" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="V14" s="5"/>
+      <c r="W14" s="5"/>
+    </row>
+    <row r="15" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -1128,7 +1177,7 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
-      <c r="M15" s="5"/>
+      <c r="K15" s="5"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
@@ -1137,8 +1186,10 @@
       <c r="S15" s="5"/>
       <c r="T15" s="5"/>
       <c r="U15" s="5"/>
-    </row>
-    <row r="16" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="V15" s="5"/>
+      <c r="W15" s="5"/>
+    </row>
+    <row r="16" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -1148,7 +1199,7 @@
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
-      <c r="M16" s="5"/>
+      <c r="K16" s="5"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
@@ -1157,8 +1208,10 @@
       <c r="S16" s="5"/>
       <c r="T16" s="5"/>
       <c r="U16" s="5"/>
-    </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V16" s="5"/>
+      <c r="W16" s="5"/>
+    </row>
+    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -1168,7 +1221,7 @@
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
-      <c r="M17" s="5"/>
+      <c r="K17" s="5"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
@@ -1177,8 +1230,10 @@
       <c r="S17" s="5"/>
       <c r="T17" s="5"/>
       <c r="U17" s="5"/>
-    </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V17" s="5"/>
+      <c r="W17" s="5"/>
+    </row>
+    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1188,7 +1243,7 @@
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
-      <c r="M18" s="5"/>
+      <c r="K18" s="5"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
@@ -1197,8 +1252,10 @@
       <c r="S18" s="5"/>
       <c r="T18" s="5"/>
       <c r="U18" s="5"/>
-    </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V18" s="5"/>
+      <c r="W18" s="5"/>
+    </row>
+    <row r="19" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -1208,7 +1265,7 @@
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
-      <c r="M19" s="5"/>
+      <c r="K19" s="5"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
@@ -1217,8 +1274,10 @@
       <c r="S19" s="5"/>
       <c r="T19" s="5"/>
       <c r="U19" s="5"/>
-    </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V19" s="5"/>
+      <c r="W19" s="5"/>
+    </row>
+    <row r="20" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -1228,7 +1287,7 @@
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
-      <c r="M20" s="5"/>
+      <c r="K20" s="5"/>
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
       <c r="P20" s="5"/>
@@ -1237,8 +1296,10 @@
       <c r="S20" s="5"/>
       <c r="T20" s="5"/>
       <c r="U20" s="5"/>
-    </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V20" s="5"/>
+      <c r="W20" s="5"/>
+    </row>
+    <row r="21" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -1248,7 +1309,7 @@
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
-      <c r="M21" s="5"/>
+      <c r="K21" s="5"/>
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
       <c r="P21" s="5"/>
@@ -1257,8 +1318,10 @@
       <c r="S21" s="5"/>
       <c r="T21" s="5"/>
       <c r="U21" s="5"/>
-    </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V21" s="5"/>
+      <c r="W21" s="5"/>
+    </row>
+    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -1268,7 +1331,7 @@
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
-      <c r="M22" s="5"/>
+      <c r="K22" s="5"/>
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
       <c r="P22" s="5"/>
@@ -1277,8 +1340,10 @@
       <c r="S22" s="5"/>
       <c r="T22" s="5"/>
       <c r="U22" s="5"/>
-    </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V22" s="5"/>
+      <c r="W22" s="5"/>
+    </row>
+    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -1288,7 +1353,7 @@
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
-      <c r="M23" s="5"/>
+      <c r="K23" s="5"/>
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
       <c r="P23" s="5"/>
@@ -1297,8 +1362,10 @@
       <c r="S23" s="5"/>
       <c r="T23" s="5"/>
       <c r="U23" s="5"/>
-    </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V23" s="5"/>
+      <c r="W23" s="5"/>
+    </row>
+    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -1308,7 +1375,7 @@
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
-      <c r="M24" s="5"/>
+      <c r="K24" s="5"/>
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
       <c r="P24" s="5"/>
@@ -1317,8 +1384,10 @@
       <c r="S24" s="5"/>
       <c r="T24" s="5"/>
       <c r="U24" s="5"/>
-    </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V24" s="5"/>
+      <c r="W24" s="5"/>
+    </row>
+    <row r="25" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
@@ -1328,7 +1397,7 @@
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
-      <c r="M25" s="5"/>
+      <c r="K25" s="5"/>
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
       <c r="P25" s="5"/>
@@ -1337,8 +1406,10 @@
       <c r="S25" s="5"/>
       <c r="T25" s="5"/>
       <c r="U25" s="5"/>
-    </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V25" s="5"/>
+      <c r="W25" s="5"/>
+    </row>
+    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -1348,7 +1419,7 @@
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
-      <c r="M26" s="5"/>
+      <c r="K26" s="5"/>
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
       <c r="P26" s="5"/>
@@ -1357,8 +1428,10 @@
       <c r="S26" s="5"/>
       <c r="T26" s="5"/>
       <c r="U26" s="5"/>
-    </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V26" s="5"/>
+      <c r="W26" s="5"/>
+    </row>
+    <row r="27" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -1368,7 +1441,7 @@
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
-      <c r="M27" s="5"/>
+      <c r="K27" s="5"/>
       <c r="N27" s="5"/>
       <c r="O27" s="5"/>
       <c r="P27" s="5"/>
@@ -1377,8 +1450,10 @@
       <c r="S27" s="5"/>
       <c r="T27" s="5"/>
       <c r="U27" s="5"/>
-    </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V27" s="5"/>
+      <c r="W27" s="5"/>
+    </row>
+    <row r="28" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -1388,7 +1463,7 @@
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
-      <c r="M28" s="5"/>
+      <c r="K28" s="5"/>
       <c r="N28" s="5"/>
       <c r="O28" s="5"/>
       <c r="P28" s="5"/>
@@ -1397,8 +1472,10 @@
       <c r="S28" s="5"/>
       <c r="T28" s="5"/>
       <c r="U28" s="5"/>
-    </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V28" s="5"/>
+      <c r="W28" s="5"/>
+    </row>
+    <row r="29" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -1408,7 +1485,7 @@
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
-      <c r="M29" s="5"/>
+      <c r="K29" s="5"/>
       <c r="N29" s="5"/>
       <c r="O29" s="5"/>
       <c r="P29" s="5"/>
@@ -1417,8 +1494,10 @@
       <c r="S29" s="5"/>
       <c r="T29" s="5"/>
       <c r="U29" s="5"/>
-    </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V29" s="5"/>
+      <c r="W29" s="5"/>
+    </row>
+    <row r="30" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -1428,7 +1507,7 @@
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
-      <c r="M30" s="5"/>
+      <c r="K30" s="5"/>
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
       <c r="P30" s="5"/>
@@ -1437,8 +1516,10 @@
       <c r="S30" s="5"/>
       <c r="T30" s="5"/>
       <c r="U30" s="5"/>
-    </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V30" s="5"/>
+      <c r="W30" s="5"/>
+    </row>
+    <row r="31" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -1448,7 +1529,7 @@
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
-      <c r="M31" s="5"/>
+      <c r="K31" s="5"/>
       <c r="N31" s="5"/>
       <c r="O31" s="5"/>
       <c r="P31" s="5"/>
@@ -1457,8 +1538,10 @@
       <c r="S31" s="5"/>
       <c r="T31" s="5"/>
       <c r="U31" s="5"/>
-    </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V31" s="5"/>
+      <c r="W31" s="5"/>
+    </row>
+    <row r="32" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -1468,7 +1551,7 @@
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
-      <c r="M32" s="5"/>
+      <c r="K32" s="5"/>
       <c r="N32" s="5"/>
       <c r="O32" s="5"/>
       <c r="P32" s="5"/>
@@ -1477,8 +1560,10 @@
       <c r="S32" s="5"/>
       <c r="T32" s="5"/>
       <c r="U32" s="5"/>
-    </row>
-    <row r="33" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="V32" s="5"/>
+      <c r="W32" s="5"/>
+    </row>
+    <row r="33" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -1488,7 +1573,7 @@
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
-      <c r="M33" s="5"/>
+      <c r="K33" s="5"/>
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
       <c r="P33" s="5"/>
@@ -1497,8 +1582,10 @@
       <c r="S33" s="5"/>
       <c r="T33" s="5"/>
       <c r="U33" s="5"/>
-    </row>
-    <row r="34" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="V33" s="5"/>
+      <c r="W33" s="5"/>
+    </row>
+    <row r="34" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -1508,7 +1595,7 @@
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
-      <c r="M34" s="5"/>
+      <c r="K34" s="5"/>
       <c r="N34" s="5"/>
       <c r="O34" s="5"/>
       <c r="P34" s="5"/>
@@ -1517,8 +1604,10 @@
       <c r="S34" s="5"/>
       <c r="T34" s="5"/>
       <c r="U34" s="5"/>
-    </row>
-    <row r="35" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="V34" s="5"/>
+      <c r="W34" s="5"/>
+    </row>
+    <row r="35" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -1528,7 +1617,7 @@
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
-      <c r="M35" s="5"/>
+      <c r="K35" s="5"/>
       <c r="N35" s="5"/>
       <c r="O35" s="5"/>
       <c r="P35" s="5"/>
@@ -1537,84 +1626,92 @@
       <c r="S35" s="5"/>
       <c r="T35" s="5"/>
       <c r="U35" s="5"/>
-    </row>
-    <row r="36" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="W36" s="16" t="s">
+      <c r="V35" s="5"/>
+      <c r="W35" s="5"/>
+    </row>
+    <row r="36" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="Y36" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="X36" s="16"/>
-    </row>
-    <row r="37" spans="2:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C37" s="17" t="s">
+      <c r="Z36" s="17"/>
+    </row>
+    <row r="37" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C37" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="17"/>
-      <c r="H37" s="17"/>
-      <c r="I37" s="17"/>
-      <c r="N37" s="17" t="s">
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="14"/>
+      <c r="O37" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="O37" s="17"/>
-      <c r="P37" s="17"/>
-      <c r="Q37" s="17"/>
-      <c r="R37" s="17"/>
-      <c r="S37" s="17"/>
-      <c r="T37" s="17"/>
-      <c r="W37" s="11" t="s">
+      <c r="P37" s="18"/>
+      <c r="Q37" s="18"/>
+      <c r="R37" s="18"/>
+      <c r="S37" s="18"/>
+      <c r="T37" s="18"/>
+      <c r="U37" s="18"/>
+      <c r="V37" s="18"/>
+      <c r="Y37" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="X37" s="9" t="s">
+      <c r="Z37" s="9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="2:24" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="17"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="17"/>
-      <c r="N38" s="17"/>
-      <c r="O38" s="17"/>
-      <c r="P38" s="17"/>
-      <c r="Q38" s="17"/>
-      <c r="R38" s="17"/>
-      <c r="S38" s="17"/>
-      <c r="T38" s="17"/>
-      <c r="W38" s="12" t="s">
+    <row r="38" spans="2:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="18"/>
+      <c r="J38" s="14"/>
+      <c r="O38" s="18"/>
+      <c r="P38" s="18"/>
+      <c r="Q38" s="18"/>
+      <c r="R38" s="18"/>
+      <c r="S38" s="18"/>
+      <c r="T38" s="18"/>
+      <c r="U38" s="18"/>
+      <c r="V38" s="18"/>
+      <c r="Y38" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="X38" s="9" t="s">
+      <c r="Z38" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="2:24" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C39" s="17"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="17"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="17"/>
-      <c r="H39" s="17"/>
-      <c r="I39" s="17"/>
-      <c r="N39" s="17"/>
-      <c r="O39" s="17"/>
-      <c r="P39" s="17"/>
-      <c r="Q39" s="17"/>
-      <c r="R39" s="17"/>
-      <c r="S39" s="17"/>
-      <c r="T39" s="17"/>
-      <c r="W39" s="12" t="s">
+    <row r="39" spans="2:26" ht="32.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="18"/>
+      <c r="J39" s="14"/>
+      <c r="O39" s="18"/>
+      <c r="P39" s="18"/>
+      <c r="Q39" s="18"/>
+      <c r="R39" s="18"/>
+      <c r="S39" s="18"/>
+      <c r="T39" s="18"/>
+      <c r="U39" s="18"/>
+      <c r="V39" s="18"/>
+      <c r="Y39" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="X39" s="9" t="s">
+      <c r="Z39" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="2:24" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:26" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>9</v>
       </c>
@@ -1630,32 +1727,33 @@
       <c r="F40" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="M40" t="s">
+      <c r="N40" t="s">
         <v>9</v>
       </c>
-      <c r="N40" s="2" t="s">
+      <c r="O40" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="O40" s="2" t="s">
+      <c r="P40" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="P40" s="2" t="s">
+      <c r="Q40" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="Q40" s="2" t="s">
+      <c r="R40" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="R40" s="13"/>
       <c r="S40" s="13"/>
-      <c r="W40" s="12" t="s">
+      <c r="T40" s="13"/>
+      <c r="U40" s="13"/>
+      <c r="Y40" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="X40" s="9" t="s">
+      <c r="Z40" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+    <row r="41" spans="2:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="5" t="s">
         <v>50</v>
       </c>
       <c r="C41" s="5" t="s">
@@ -1670,32 +1768,33 @@
       <c r="F41" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="M41" s="5" t="s">
+      <c r="N41" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="N41" s="5" t="s">
+      <c r="O41" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="O41" s="5">
+      <c r="P41" s="5">
         <v>300</v>
       </c>
-      <c r="P41" s="5">
+      <c r="Q41" s="5">
         <v>0</v>
       </c>
-      <c r="Q41" s="8" t="s">
+      <c r="R41" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="R41" s="10"/>
       <c r="S41" s="10"/>
-      <c r="W41" s="11" t="s">
+      <c r="T41" s="10"/>
+      <c r="U41" s="10"/>
+      <c r="Y41" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="X41" s="9" t="s">
+      <c r="Z41" s="9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+    <row r="42" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B42" s="5" t="s">
         <v>47</v>
       </c>
       <c r="C42" s="5" t="s">
@@ -1710,198 +1809,217 @@
       <c r="F42" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M42" s="5" t="s">
+      <c r="N42" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="N42" s="5" t="s">
+      <c r="O42" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="O42" s="5">
+      <c r="P42" s="5">
         <v>15</v>
       </c>
-      <c r="P42" s="5">
+      <c r="Q42" s="5">
         <v>0</v>
       </c>
-      <c r="Q42" s="8" t="s">
+      <c r="R42" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="R42" s="10"/>
       <c r="S42" s="10"/>
-      <c r="W42" s="11" t="s">
+      <c r="T42" s="10"/>
+      <c r="U42" s="10"/>
+      <c r="Y42" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="X42" s="9" t="s">
+      <c r="Z42" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
-      <c r="M43" s="5"/>
       <c r="N43" s="5"/>
       <c r="O43" s="5"/>
       <c r="P43" s="5"/>
       <c r="Q43" s="5"/>
-      <c r="R43" s="7"/>
+      <c r="R43" s="5"/>
       <c r="S43" s="7"/>
-      <c r="W43" s="12" t="s">
+      <c r="T43" s="7"/>
+      <c r="U43" s="7"/>
+      <c r="Y43" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="X43" s="9" t="s">
+      <c r="Z43" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
-      <c r="M44" s="5"/>
       <c r="N44" s="5"/>
       <c r="O44" s="5"/>
       <c r="P44" s="5"/>
       <c r="Q44" s="5"/>
-      <c r="R44" s="7"/>
+      <c r="R44" s="5"/>
       <c r="S44" s="7"/>
-      <c r="W44" s="6" t="s">
+      <c r="T44" s="7"/>
+      <c r="U44" s="7"/>
+      <c r="Y44" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="X44" s="9" t="s">
+      <c r="Z44" s="9" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
-      <c r="M45" s="5"/>
       <c r="N45" s="5"/>
       <c r="O45" s="5"/>
       <c r="P45" s="5"/>
       <c r="Q45" s="5"/>
-      <c r="R45" s="7"/>
+      <c r="R45" s="5"/>
       <c r="S45" s="7"/>
-      <c r="W45" s="7"/>
-      <c r="X45" s="10"/>
-    </row>
-    <row r="46" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="T45" s="7"/>
+      <c r="U45" s="7"/>
+      <c r="Y45" s="7"/>
+      <c r="Z45" s="10"/>
+    </row>
+    <row r="46" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
-      <c r="M46" s="5"/>
       <c r="N46" s="5"/>
       <c r="O46" s="5"/>
       <c r="P46" s="5"/>
       <c r="Q46" s="5"/>
-      <c r="R46" s="7"/>
+      <c r="R46" s="5"/>
       <c r="S46" s="7"/>
-      <c r="W46" s="7"/>
-      <c r="X46" s="10"/>
-    </row>
-    <row r="47" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="T46" s="7"/>
+      <c r="U46" s="7"/>
+      <c r="Y46" s="7"/>
+      <c r="Z46" s="10"/>
+    </row>
+    <row r="47" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
-      <c r="M47" s="5"/>
       <c r="N47" s="5"/>
       <c r="O47" s="5"/>
       <c r="P47" s="5"/>
       <c r="Q47" s="5"/>
-      <c r="R47" s="7"/>
+      <c r="R47" s="5"/>
       <c r="S47" s="7"/>
-      <c r="W47" s="7"/>
-      <c r="X47" s="10"/>
-    </row>
-    <row r="48" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="T47" s="7"/>
+      <c r="U47" s="7"/>
+      <c r="Y47" s="7"/>
+      <c r="Z47" s="10"/>
+    </row>
+    <row r="48" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
-      <c r="M48" s="5"/>
       <c r="N48" s="5"/>
       <c r="O48" s="5"/>
       <c r="P48" s="5"/>
       <c r="Q48" s="5"/>
-      <c r="R48" s="7"/>
+      <c r="R48" s="5"/>
       <c r="S48" s="7"/>
-    </row>
-    <row r="49" spans="3:24" x14ac:dyDescent="0.25">
+      <c r="T48" s="7"/>
+      <c r="U48" s="7"/>
+    </row>
+    <row r="49" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
-      <c r="M49" s="5"/>
       <c r="N49" s="5"/>
       <c r="O49" s="5"/>
       <c r="P49" s="5"/>
       <c r="Q49" s="5"/>
-      <c r="R49" s="7"/>
+      <c r="R49" s="5"/>
       <c r="S49" s="7"/>
-      <c r="W49" s="6" t="s">
+      <c r="T49" s="7"/>
+      <c r="U49" s="7"/>
+      <c r="Y49" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="X49" s="9" t="s">
+      <c r="Z49" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
-      <c r="M50" s="5"/>
       <c r="N50" s="5"/>
       <c r="O50" s="5"/>
       <c r="P50" s="5"/>
       <c r="Q50" s="5"/>
-      <c r="R50" s="7"/>
+      <c r="R50" s="5"/>
       <c r="S50" s="7"/>
-      <c r="W50" s="6" t="s">
+      <c r="T50" s="7"/>
+      <c r="U50" s="7"/>
+      <c r="Y50" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="X50" s="9" t="s">
+      <c r="Z50" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="51" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
-      <c r="M51" s="5"/>
       <c r="N51" s="5"/>
       <c r="O51" s="5"/>
       <c r="P51" s="5"/>
       <c r="Q51" s="5"/>
-      <c r="R51" s="7"/>
+      <c r="R51" s="5"/>
       <c r="S51" s="7"/>
-      <c r="W51" s="6" t="s">
+      <c r="T51" s="7"/>
+      <c r="U51" s="7"/>
+      <c r="Y51" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="X51" s="9" t="s">
+      <c r="Z51" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="W52" s="6" t="s">
+    <row r="52" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="Y52" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="X52" s="9" t="s">
+      <c r="Z52" s="9" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="W1:Y2"/>
-    <mergeCell ref="N1:U2"/>
-    <mergeCell ref="C1:J2"/>
-    <mergeCell ref="W36:X36"/>
-    <mergeCell ref="N37:T39"/>
+    <mergeCell ref="Y1:AA2"/>
+    <mergeCell ref="O1:W2"/>
+    <mergeCell ref="C1:K2"/>
+    <mergeCell ref="Y36:Z36"/>
+    <mergeCell ref="O37:V39"/>
     <mergeCell ref="C37:I39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
some fix magic and abil
</commit_message>
<xml_diff>
--- a/BattleScript/table.xlsx
+++ b/BattleScript/table.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0811E3A9-3A4A-4951-9F1D-76DBA6804EA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -219,7 +220,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -627,11 +628,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AA52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V9" sqref="V9"/>
+      <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -907,7 +908,7 @@
         <v>21</v>
       </c>
       <c r="V5" s="5">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="W5" s="5">
         <v>10</v>
@@ -1760,13 +1761,13 @@
         <v>36</v>
       </c>
       <c r="D41" s="5">
-        <v>500</v>
+        <v>800</v>
       </c>
       <c r="E41" s="5">
         <v>0</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="N41" s="5" t="s">
         <v>62</v>
@@ -1775,13 +1776,13 @@
         <v>36</v>
       </c>
       <c r="P41" s="5">
-        <v>300</v>
+        <v>800</v>
       </c>
       <c r="Q41" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R41" s="8" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="S41" s="10"/>
       <c r="T41" s="10"/>
@@ -1807,7 +1808,7 @@
         <v>0</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="N42" s="5" t="s">
         <v>63</v>
@@ -1822,7 +1823,7 @@
         <v>0</v>
       </c>
       <c r="R42" s="8" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="S42" s="10"/>
       <c r="T42" s="10"/>

</xml_diff>

<commit_message>
fix bug with Nonetype in targets field
</commit_message>
<xml_diff>
--- a/BattleScript/table.xlsx
+++ b/BattleScript/table.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA94E671-4184-4834-8757-4FF64AD905CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
   <si>
     <t>Армия первая</t>
   </si>
@@ -128,12 +127,15 @@
   </si>
   <si>
     <t>Бонус к комбатке</t>
+  </si>
+  <si>
+    <t>т2 конница</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -499,11 +501,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AA41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,7 +686,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N4" s="5" t="s">
         <v>10</v>
@@ -782,7 +784,7 @@
         <v>90</v>
       </c>
       <c r="W5" s="5">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="Z5" s="6" t="s">
         <v>24</v>
@@ -799,7 +801,7 @@
         <v>19</v>
       </c>
       <c r="D6" s="5">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="E6" s="5">
         <v>900</v>
@@ -820,18 +822,38 @@
         <v>0</v>
       </c>
       <c r="K6" s="5">
+        <v>1</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="P6" s="5">
+        <v>250</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>250</v>
+      </c>
+      <c r="R6" s="5">
+        <v>10</v>
+      </c>
+      <c r="S6" s="5">
+        <v>10</v>
+      </c>
+      <c r="T6" s="5">
+        <v>0</v>
+      </c>
+      <c r="U6" s="5">
+        <v>0</v>
+      </c>
+      <c r="V6" s="5">
+        <v>25</v>
+      </c>
+      <c r="W6" s="5">
         <v>2</v>
       </c>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5"/>
-      <c r="U6" s="5"/>
-      <c r="V6" s="5"/>
-      <c r="W6" s="5"/>
       <c r="Z6" s="6" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
added statistics about casualties in population after battle in file_writer and main_logic functions
</commit_message>
<xml_diff>
--- a/BattleScript/table.xlsx
+++ b/BattleScript/table.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93649B3-04A7-4EA2-85C4-801325250AFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -120,7 +121,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -486,11 +487,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AA41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,7 +651,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="5">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E4" s="5">
         <v>100</v>
@@ -671,7 +672,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N4" s="5" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
extended statistics after battle
</commit_message>
<xml_diff>
--- a/BattleScript/table.xlsx
+++ b/BattleScript/table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93649B3-04A7-4EA2-85C4-801325250AFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C30FB3F-4264-479E-8671-0DE321516407}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -112,10 +112,10 @@
     <t>Бонус к комбатке</t>
   </si>
   <si>
-    <t>Govno</t>
-  </si>
-  <si>
-    <t>Mocha</t>
+    <t>Potato_Low_dick</t>
+  </si>
+  <si>
+    <t>Potato_big_ass</t>
   </si>
 </sst>
 </file>
@@ -491,7 +491,7 @@
   <dimension ref="B1:AA41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added statistics about dead units and morale modifier
</commit_message>
<xml_diff>
--- a/BattleScript/table.xlsx
+++ b/BattleScript/table.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C30FB3F-4264-479E-8671-0DE321516407}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <t>Армия первая</t>
   </si>
@@ -94,9 +93,6 @@
     <t>полководец</t>
   </si>
   <si>
-    <t>особый</t>
-  </si>
-  <si>
     <t>Комбатка макс.</t>
   </si>
   <si>
@@ -116,12 +112,21 @@
   </si>
   <si>
     <t>Potato_big_ass</t>
+  </si>
+  <si>
+    <t>к+в</t>
+  </si>
+  <si>
+    <t>одиночный</t>
+  </si>
+  <si>
+    <t>Геныч</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -487,11 +492,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AA41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,10 +588,10 @@
         <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="F3" t="s">
         <v>1</v>
@@ -601,7 +606,7 @@
         <v>10</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>5</v>
@@ -613,10 +618,10 @@
         <v>4</v>
       </c>
       <c r="P3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q3" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="R3" t="s">
         <v>1</v>
@@ -631,10 +636,10 @@
         <v>10</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Z3" s="6" t="s">
         <v>6</v>
@@ -645,7 +650,7 @@
     </row>
     <row r="4" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>11</v>
@@ -657,7 +662,7 @@
         <v>100</v>
       </c>
       <c r="F4" s="5">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="G4" s="5">
         <v>0</v>
@@ -666,16 +671,16 @@
         <v>0</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="J4" s="5">
         <v>0</v>
       </c>
       <c r="K4" s="5">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O4" s="5" t="s">
         <v>11</v>
@@ -693,7 +698,7 @@
         <v>0</v>
       </c>
       <c r="T4" s="5">
-        <v>-50</v>
+        <v>-90</v>
       </c>
       <c r="U4" s="5" t="s">
         <v>13</v>
@@ -702,7 +707,7 @@
         <v>0</v>
       </c>
       <c r="W4" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Z4" s="6" t="s">
         <v>7</v>
@@ -722,16 +727,34 @@
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
+      <c r="N5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="P5" s="5">
+        <v>25</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>25</v>
+      </c>
+      <c r="R5" s="5">
+        <v>0</v>
+      </c>
+      <c r="S5" s="5">
+        <v>0</v>
+      </c>
+      <c r="T5" s="5">
+        <v>-90</v>
+      </c>
       <c r="U5" s="5"/>
-      <c r="V5" s="5"/>
-      <c r="W5" s="5"/>
+      <c r="V5" s="5">
+        <v>0</v>
+      </c>
+      <c r="W5" s="5">
+        <v>1</v>
+      </c>
       <c r="Z5" s="6" t="s">
         <v>19</v>
       </c>
@@ -792,7 +815,7 @@
         <v>21</v>
       </c>
       <c r="AA7" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="2:27" x14ac:dyDescent="0.25">
@@ -873,7 +896,7 @@
       <c r="V10" s="5"/>
       <c r="W10" s="5"/>
       <c r="Z10" s="6" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="AA10" s="6" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
swap copy to deepcopy, add requeriments, delete temp result.txt + get nostatgic
</commit_message>
<xml_diff>
--- a/BattleScript/table.xlsx
+++ b/BattleScript/table.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2BF183-D55B-41B9-BAD6-984E79865671}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t>Армия первая</t>
   </si>
@@ -108,25 +109,22 @@
     <t>Бонус к комбатке</t>
   </si>
   <si>
-    <t>Potato_Low_dick</t>
-  </si>
-  <si>
-    <t>Potato_big_ass</t>
-  </si>
-  <si>
     <t>к+в</t>
   </si>
   <si>
     <t>одиночный</t>
   </si>
   <si>
-    <t>Геныч</t>
+    <t>unit_by_default</t>
+  </si>
+  <si>
+    <t>general_by_default</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -195,7 +193,7 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -492,11 +490,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AA41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,7 +648,7 @@
     </row>
     <row r="4" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>11</v>
@@ -671,7 +669,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J4" s="5">
         <v>0</v>
@@ -680,7 +678,7 @@
         <v>3</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O4" s="5" t="s">
         <v>11</v>
@@ -728,7 +726,7 @@
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
       <c r="N5" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O5" s="5" t="s">
         <v>16</v>
@@ -896,7 +894,7 @@
       <c r="V10" s="5"/>
       <c r="W10" s="5"/>
       <c r="Z10" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="AA10" s="6" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
add README.md + some changes in excel-file
</commit_message>
<xml_diff>
--- a/BattleScript/table.xlsx
+++ b/BattleScript/table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2BF183-D55B-41B9-BAD6-984E79865671}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26B0FED-5C94-4F53-9A80-5A790DD0C004}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -115,10 +115,10 @@
     <t>одиночный</t>
   </si>
   <si>
-    <t>unit_by_default</t>
-  </si>
-  <si>
-    <t>general_by_default</t>
+    <t>default_unit</t>
+  </si>
+  <si>
+    <t>default_general</t>
   </si>
 </sst>
 </file>
@@ -494,7 +494,7 @@
   <dimension ref="B1:AA41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,21 +502,21 @@
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
     <col min="4" max="5" width="9.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
     <col min="10" max="10" width="11.28515625" customWidth="1"/>
     <col min="11" max="11" width="11.42578125" customWidth="1"/>
     <col min="12" max="12" width="4.28515625" customWidth="1"/>
     <col min="13" max="13" width="4.7109375" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" customWidth="1"/>
     <col min="15" max="15" width="9.7109375" customWidth="1"/>
     <col min="16" max="17" width="10" customWidth="1"/>
-    <col min="18" max="18" width="17.140625" customWidth="1"/>
-    <col min="19" max="20" width="12.5703125" customWidth="1"/>
-    <col min="21" max="21" width="9.7109375" customWidth="1"/>
-    <col min="22" max="22" width="14.85546875" customWidth="1"/>
-    <col min="23" max="23" width="13.42578125" customWidth="1"/>
+    <col min="18" max="19" width="11" customWidth="1"/>
+    <col min="20" max="20" width="8.42578125" customWidth="1"/>
+    <col min="21" max="21" width="8" customWidth="1"/>
+    <col min="22" max="22" width="10.140625" customWidth="1"/>
+    <col min="23" max="23" width="10.28515625" customWidth="1"/>
     <col min="24" max="24" width="3.85546875" customWidth="1"/>
     <col min="25" max="25" width="15.28515625" customWidth="1"/>
     <col min="26" max="26" width="12" customWidth="1"/>
@@ -591,7 +591,7 @@
       <c r="E3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -621,7 +621,7 @@
       <c r="Q3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="R3" t="s">
+      <c r="R3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="S3" s="2" t="s">

</xml_diff>

<commit_message>
massive refactoring2, added some comments, first and second stage functions unite in classes
</commit_message>
<xml_diff>
--- a/BattleScript/table.xlsx
+++ b/BattleScript/table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26B0FED-5C94-4F53-9A80-5A790DD0C004}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD6B61BD-38D0-4E17-A93F-D7A7A6ECA7B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -494,7 +494,7 @@
   <dimension ref="B1:AA41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,7 +705,7 @@
         <v>0</v>
       </c>
       <c r="W4" s="5">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="Z4" s="6" t="s">
         <v>7</v>

</xml_diff>